<commit_message>
pattabhi - modifieed schedulers
</commit_message>
<xml_diff>
--- a/public/Payroll/October-2014-payslips.xlsx
+++ b/public/Payroll/October-2014-payslips.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -75,33 +75,26 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.989887640449439"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.18988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.88988764044944"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.989887640449439"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.08988764044944"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.88988764044944"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.48988764044944"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="4.189887640449439"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="9.68988764044944"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -172,80 +165,45 @@
       </c>
       <c r="N1" s="0" t="inlineStr">
         <is>
-          <t>ABC1</t>
+          <t>Spcl Allowance</t>
         </is>
       </c>
       <c r="O1" s="0" t="inlineStr">
         <is>
-          <t>Abc12</t>
+          <t>Arrears</t>
         </is>
       </c>
       <c r="P1" s="0" t="inlineStr">
         <is>
-          <t>Ab</t>
+          <t>Gross Pay</t>
         </is>
       </c>
       <c r="Q1" s="0" t="inlineStr">
         <is>
-          <t>aa1</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="R1" s="0" t="inlineStr">
         <is>
-          <t>Spcl Allowance</t>
+          <t>ESIC</t>
         </is>
       </c>
       <c r="S1" s="0" t="inlineStr">
         <is>
-          <t>Arrears</t>
+          <t>PT</t>
         </is>
       </c>
       <c r="T1" s="0" t="inlineStr">
         <is>
-          <t>Gross Pay</t>
+          <t>TDS</t>
         </is>
       </c>
       <c r="U1" s="0" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>total_deducations</t>
         </is>
       </c>
       <c r="V1" s="0" t="inlineStr">
-        <is>
-          <t>ESIC</t>
-        </is>
-      </c>
-      <c r="W1" s="0" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="X1" s="0" t="inlineStr">
-        <is>
-          <t>TDS</t>
-        </is>
-      </c>
-      <c r="Y1" s="0" t="inlineStr">
-        <is>
-          <t>ABC</t>
-        </is>
-      </c>
-      <c r="Z1" s="0" t="inlineStr">
-        <is>
-          <t>aaaaaa</t>
-        </is>
-      </c>
-      <c r="AA1" s="0" t="inlineStr">
-        <is>
-          <t>XYZ</t>
-        </is>
-      </c>
-      <c r="AB1" s="0" t="inlineStr">
-        <is>
-          <t>total_deducations</t>
-        </is>
-      </c>
-      <c r="AC1" s="0" t="inlineStr">
         <is>
           <t>NetPay</t>
         </is>
@@ -262,7 +220,7 @@
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>Sekhar Beri</t>
+          <t>Vidya Sagar  Pogiri</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
@@ -277,12 +235,12 @@
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>Junior HR</t>
+          <t>Junior Development</t>
         </is>
       </c>
       <c r="G2" s="0" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>Development</t>
         </is>
       </c>
       <c r="H2" s="0" t="n">
@@ -292,7 +250,7 @@
         <v>10000.0</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>9520.0</v>
+        <v>10000.0</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>31.0</v>
@@ -304,52 +262,31 @@
         <v>4000.0</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>0</v>
+        <v>6000.0</v>
       </c>
       <c r="O2" s="0" t="n">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="P2" s="0" t="n">
-        <v>0</v>
+        <v>10000.0</v>
       </c>
       <c r="Q2" s="0" t="n">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="R2" s="0" t="n">
-        <v>5520.0</v>
+        <v>0.0</v>
       </c>
       <c r="S2" s="0" t="n">
         <v>0.0</v>
       </c>
       <c r="T2" s="0" t="n">
-        <v>9520.0</v>
+        <v>0.0</v>
       </c>
       <c r="U2" s="0" t="n">
-        <v>480.0</v>
+        <v>0.0</v>
       </c>
       <c r="V2" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W2" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="X2" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Y2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="0" t="n">
-        <v>480.0</v>
-      </c>
-      <c r="AC2" s="0" t="n">
-        <v>9040.0</v>
+        <v>10000.0</v>
       </c>
     </row>
     <row r="3">
@@ -378,12 +315,12 @@
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>Junior HR</t>
+          <t>Junior Accounts</t>
         </is>
       </c>
       <c r="G3" s="0" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>Accounts</t>
         </is>
       </c>
       <c r="H3" s="0" t="n">
@@ -393,7 +330,7 @@
         <v>10000.0</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>9371.0</v>
+        <v>10000.0</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>31.0</v>
@@ -405,52 +342,31 @@
         <v>4000.0</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>440.0</v>
+        <v>6000.0</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>40.0</v>
+        <v>10000.0</v>
       </c>
       <c r="Q3" s="0" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="R3" s="0" t="n">
-        <v>4811.0</v>
+        <v>0.0</v>
       </c>
       <c r="S3" s="0" t="n">
-        <v>1000.0</v>
+        <v>0.0</v>
       </c>
       <c r="T3" s="0" t="n">
-        <v>9371.0</v>
+        <v>0.0</v>
       </c>
       <c r="U3" s="0" t="n">
-        <v>480.0</v>
+        <v>0.0</v>
       </c>
       <c r="V3" s="0" t="n">
-        <v>163.99</v>
-      </c>
-      <c r="W3" s="0" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="X3" s="0" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="Y3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="0" t="n">
-        <v>1069.99</v>
-      </c>
-      <c r="AC3" s="0" t="n">
-        <v>9301.01</v>
+        <v>10000.0</v>
       </c>
     </row>
     <row r="4">
@@ -479,12 +395,12 @@
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t>Junior HR</t>
+          <t>Junior Business Development</t>
         </is>
       </c>
       <c r="G4" s="0" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>Business Development</t>
         </is>
       </c>
       <c r="H4" s="0" t="n">
@@ -494,7 +410,7 @@
         <v>10000.0</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>9345.0</v>
+        <v>10000.0</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>31.0</v>
@@ -506,52 +422,31 @@
         <v>4000.0</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>0</v>
+        <v>6000.0</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>0</v>
+        <v>10000.0</v>
       </c>
       <c r="Q4" s="0" t="n">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="R4" s="0" t="n">
-        <v>5345.0</v>
+        <v>0.0</v>
       </c>
       <c r="S4" s="0" t="n">
         <v>0.0</v>
       </c>
       <c r="T4" s="0" t="n">
-        <v>9345.0</v>
+        <v>0.0</v>
       </c>
       <c r="U4" s="0" t="n">
-        <v>480.0</v>
+        <v>0.0</v>
       </c>
       <c r="V4" s="0" t="n">
-        <v>163.54</v>
-      </c>
-      <c r="W4" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="X4" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Y4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="0" t="n">
-        <v>643.54</v>
-      </c>
-      <c r="AC4" s="0" t="n">
-        <v>8701.46</v>
+        <v>10000.0</v>
       </c>
     </row>
     <row r="5">
@@ -580,12 +475,12 @@
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
-          <t>Junior Accounts</t>
+          <t>Junior HR</t>
         </is>
       </c>
       <c r="G5" s="0" t="inlineStr">
         <is>
-          <t>Accounts</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="H5" s="0" t="n">
@@ -595,7 +490,7 @@
         <v>10000.0</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>9346.0</v>
+        <v>10000.0</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>31.0</v>
@@ -607,52 +502,31 @@
         <v>4000.0</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>440.0</v>
+        <v>6000.0</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>0</v>
+        <v>10000.0</v>
       </c>
       <c r="Q5" s="0" t="n">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="R5" s="0" t="n">
-        <v>4906.0</v>
+        <v>0.0</v>
       </c>
       <c r="S5" s="0" t="n">
         <v>0.0</v>
       </c>
       <c r="T5" s="0" t="n">
-        <v>9346.0</v>
+        <v>0.0</v>
       </c>
       <c r="U5" s="0" t="n">
-        <v>480.0</v>
+        <v>0.0</v>
       </c>
       <c r="V5" s="0" t="n">
-        <v>163.56</v>
-      </c>
-      <c r="W5" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="X5" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Y5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="0" t="n">
-        <v>644.56</v>
-      </c>
-      <c r="AC5" s="0" t="n">
-        <v>8701.44</v>
+        <v>10000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Balaraju -added code for SALAry
</commit_message>
<xml_diff>
--- a/public/Payroll/October-2014-payslips.xlsx
+++ b/public/Payroll/October-2014-payslips.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -75,34 +75,30 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.989887640449439"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.88988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.28988764044944"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.989887640449439"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="14.08988764044944"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.78988764044944"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.989887640449439"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="21.789887640449443"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.78988764044944"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="18.48988764044944"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="5.289887640449439"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="5.289887640449439"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="12.989887640449439"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="14.08988764044944"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="16.28988764044944"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="16.28988764044944"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="10.78988764044944"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="10.78988764044944"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.78988764044944"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.78988764044944"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="10.78988764044944"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="12.989887640449439"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="11.88988764044944"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -178,80 +174,60 @@
       </c>
       <c r="O1" s="0" t="inlineStr">
         <is>
-          <t>DA</t>
+          <t>ABC1</t>
         </is>
       </c>
       <c r="P1" s="0" t="inlineStr">
         <is>
-          <t>Travelling Allowance</t>
+          <t>Abc12</t>
         </is>
       </c>
       <c r="Q1" s="0" t="inlineStr">
         <is>
-          <t>Conveyance Allowance</t>
+          <t>Spcl Allowance</t>
         </is>
       </c>
       <c r="R1" s="0" t="inlineStr">
         <is>
-          <t>Spcl Allowance</t>
+          <t>Arrears</t>
         </is>
       </c>
       <c r="S1" s="0" t="inlineStr">
         <is>
-          <t>Arrears</t>
+          <t>Gross Pay</t>
         </is>
       </c>
       <c r="T1" s="0" t="inlineStr">
         <is>
-          <t>Gross Pay</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="U1" s="0" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>ESIC</t>
         </is>
       </c>
       <c r="V1" s="0" t="inlineStr">
         <is>
-          <t>ESIC</t>
+          <t>PT</t>
         </is>
       </c>
       <c r="W1" s="0" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>TDS</t>
         </is>
       </c>
       <c r="X1" s="0" t="inlineStr">
         <is>
-          <t>TDS</t>
+          <t>Deductible Arrears</t>
         </is>
       </c>
       <c r="Y1" s="0" t="inlineStr">
         <is>
-          <t>Deductible Arrears</t>
+          <t>total_deducations</t>
         </is>
       </c>
       <c r="Z1" s="0" t="inlineStr">
-        <is>
-          <t>Food Coupons</t>
-        </is>
-      </c>
-      <c r="AA1" s="0" t="inlineStr">
-        <is>
-          <t>Deducted allowance1</t>
-        </is>
-      </c>
-      <c r="AB1" s="0" t="inlineStr">
-        <is>
-          <t>Deducted allowance2</t>
-        </is>
-      </c>
-      <c r="AC1" s="0" t="inlineStr">
-        <is>
-          <t>total_deducations</t>
-        </is>
-      </c>
-      <c r="AD1" s="0" t="inlineStr">
         <is>
           <t>NetPay</t>
         </is>
@@ -268,17 +244,17 @@
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>Sekhar Beri</t>
+          <t>balaraju Vankala</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>02/06/2014</t>
+          <t>27/11/2014</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>Regular</t>
+          <t>New</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
@@ -292,13 +268,13 @@
         </is>
       </c>
       <c r="H2" s="0" t="n">
-        <v>120000.0</v>
+        <v>25000000.0</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>10000.0</v>
+        <v>2083333.3333333333</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>9345.0</v>
+        <v>1946880.0</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>31.0</v>
@@ -307,34 +283,34 @@
         <v>31.0</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>4000.0</v>
+        <v>833333.0</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>1000.0</v>
+        <v>208333.0</v>
       </c>
       <c r="O2" s="0" t="n">
-        <v>800.0</v>
+        <v>100000.0</v>
       </c>
       <c r="P2" s="0" t="n">
-        <v>800.0</v>
+        <v>100000.0</v>
       </c>
       <c r="Q2" s="0" t="n">
-        <v>0</v>
+        <v>705208.0</v>
       </c>
       <c r="R2" s="0" t="n">
-        <v>2745.0</v>
+        <v>0.0</v>
       </c>
       <c r="S2" s="0" t="n">
-        <v>0.0</v>
+        <v>1946880.0</v>
       </c>
       <c r="T2" s="0" t="n">
-        <v>9345.0</v>
+        <v>100000.0</v>
       </c>
       <c r="U2" s="0" t="n">
-        <v>480.0</v>
+        <v>34070.3</v>
       </c>
       <c r="V2" s="0" t="n">
-        <v>163.54</v>
+        <v>0.0</v>
       </c>
       <c r="W2" s="0" t="n">
         <v>0.0</v>
@@ -343,22 +319,10 @@
         <v>0.0</v>
       </c>
       <c r="Y2" s="0" t="n">
-        <v>0.0</v>
+        <v>134070.0</v>
       </c>
       <c r="Z2" s="0" t="n">
-        <v>2500.0</v>
-      </c>
-      <c r="AA2" s="0" t="n">
-        <v>1250.0</v>
-      </c>
-      <c r="AB2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="0" t="n">
-        <v>4393.54</v>
-      </c>
-      <c r="AD2" s="0" t="n">
-        <v>4951.46</v>
+        <v>1812800.0</v>
       </c>
     </row>
     <row r="3">
@@ -372,37 +336,37 @@
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>Priyanka Muddana</t>
+          <t>Balaraju vankala</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>02/06/2014</t>
+          <t>2014-03-03</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>Regular</t>
+          <t>New</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>Senior Developer</t>
+          <t>HR Manager</t>
         </is>
       </c>
       <c r="G3" s="0" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="H3" s="0" t="n">
-        <v>200000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>16666.666666666668</v>
+        <v>10000.0</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>15575.0</v>
+        <v>9345.0</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>31.0</v>
@@ -411,34 +375,34 @@
         <v>31.0</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>6666.67</v>
+        <v>4000.0</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>1666.67</v>
+        <v>1000.0</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>1333.33</v>
+        <v>480.0</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>1333.33</v>
+        <v>480.0</v>
       </c>
       <c r="Q3" s="0" t="n">
-        <v>1666.67</v>
+        <v>3385.0</v>
       </c>
       <c r="R3" s="0" t="n">
-        <v>2908.33</v>
+        <v>0.0</v>
       </c>
       <c r="S3" s="0" t="n">
-        <v>0.0</v>
+        <v>9345.0</v>
       </c>
       <c r="T3" s="0" t="n">
-        <v>15575.0</v>
+        <v>480.0</v>
       </c>
       <c r="U3" s="0" t="n">
-        <v>800.0</v>
+        <v>163.54</v>
       </c>
       <c r="V3" s="0" t="n">
-        <v>272.56</v>
+        <v>0.0</v>
       </c>
       <c r="W3" s="0" t="n">
         <v>0.0</v>
@@ -447,22 +411,10 @@
         <v>0.0</v>
       </c>
       <c r="Y3" s="0" t="n">
-        <v>0.0</v>
+        <v>643.54</v>
       </c>
       <c r="Z3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="0" t="n">
-        <v>1250.0</v>
-      </c>
-      <c r="AB3" s="0" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="AC3" s="0" t="n">
-        <v>3322.56</v>
-      </c>
-      <c r="AD3" s="0" t="n">
-        <v>12252.4</v>
+        <v>8701.46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>